<commit_message>
fixed budget summary, added budget card at the top
</commit_message>
<xml_diff>
--- a/Budget Template.xlsx
+++ b/Budget Template.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Timmy\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Timmy\LocalFiles\Coding\koala-budget-UAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F58E69E-08E4-42E0-BEE1-44FFF90EEAAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328345AC-A96A-4A8C-834B-BBC27C6EACDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4FB47142-1B3D-449D-828A-9AE39AA5D3D9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="20">
   <si>
     <t>Income</t>
   </si>
@@ -492,11 +493,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{694B896C-C978-4FD0-BD99-54B4F06701F3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD900E71-44FA-4EF7-9DB8-8F023E720EEC}">
   <dimension ref="B1:T15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+      <selection activeCell="I4" sqref="H3:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -568,8 +569,8 @@
         <v>6</v>
       </c>
       <c r="I3" s="4">
-        <f>SUMIF(G$14:G$24,"Asset",I$14:I$24)-SUMIF(H$14:H$24,"Asset",I$14:I$24)+D3</f>
-        <v>48500</v>
+        <f>J10-H10</f>
+        <v>47000</v>
       </c>
       <c r="J3" s="4"/>
       <c r="L3" s="6"/>
@@ -578,7 +579,7 @@
       </c>
       <c r="N3" s="6">
         <f>SUMIF(L$14:L$24,"Asset",N$14:N$24)-SUMIF(M$14:M$24,"Asset",N$14:N$24)+I3</f>
-        <v>49000</v>
+        <v>47500</v>
       </c>
       <c r="O3" s="6"/>
       <c r="Q3" s="8"/>
@@ -587,7 +588,7 @@
       </c>
       <c r="S3" s="8">
         <f>SUMIF(Q$14:Q$24,"Asset",S$14:S$24)-SUMIF(R$14:R$24,"Asset",S$14:S$24)+N3</f>
-        <v>49000</v>
+        <v>47500</v>
       </c>
       <c r="T3" s="8"/>
     </row>
@@ -607,7 +608,7 @@
       </c>
       <c r="I4" s="4">
         <f>I3-J10</f>
-        <v>0</v>
+        <v>-500</v>
       </c>
       <c r="J4" s="4"/>
       <c r="L4" s="6"/>
@@ -616,7 +617,7 @@
       </c>
       <c r="N4" s="6">
         <f>N3-O10</f>
-        <v>0</v>
+        <v>-500</v>
       </c>
       <c r="O4" s="6"/>
       <c r="Q4" s="8"/>
@@ -625,7 +626,7 @@
       </c>
       <c r="S4" s="8">
         <f>S3-T10</f>
-        <v>0</v>
+        <v>-500</v>
       </c>
       <c r="T4" s="8"/>
     </row>
@@ -708,15 +709,15 @@
         <v>0</v>
       </c>
       <c r="H7" s="4">
-        <v>0</v>
+        <v>-1500</v>
       </c>
       <c r="I7" s="4">
         <f>SUMIF(G$14:G$24,G7,I$14:I$24)-SUMIF(H$14:H$24,G7,I$14:I$24)</f>
-        <v>-1500</v>
+        <v>-1000</v>
       </c>
       <c r="J7" s="4">
         <f>H7-I7+E7</f>
-        <v>1500</v>
+        <v>-500</v>
       </c>
       <c r="L7" s="6" t="s">
         <v>0</v>
@@ -730,7 +731,7 @@
       </c>
       <c r="O7" s="6">
         <f>M7-N7+J7</f>
-        <v>1000</v>
+        <v>-1000</v>
       </c>
       <c r="Q7" s="8" t="s">
         <v>0</v>
@@ -744,7 +745,7 @@
       </c>
       <c r="T7" s="8">
         <f>R7-S7+O7</f>
-        <v>1000</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.3">
@@ -766,7 +767,7 @@
         <v>14</v>
       </c>
       <c r="H8" s="4">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="I8" s="4">
         <f>SUMIF(G$14:G$24,G8,I$14:I$24)-SUMIF(H$14:H$24,G8,I$14:I$24)</f>
@@ -774,7 +775,7 @@
       </c>
       <c r="J8" s="4">
         <f t="shared" ref="J8:J9" si="0">H8-I8+E8</f>
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="L8" s="6" t="s">
         <v>14</v>
@@ -788,7 +789,7 @@
       </c>
       <c r="O8" s="6">
         <f t="shared" ref="O8:O9" si="1">M8-N8+J8</f>
-        <v>-1000</v>
+        <v>-500</v>
       </c>
       <c r="Q8" s="8" t="s">
         <v>14</v>
@@ -802,7 +803,7 @@
       </c>
       <c r="T8" s="8">
         <f t="shared" ref="T8:T9" si="2">R8-S8+O8</f>
-        <v>-1000</v>
+        <v>-500</v>
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.3">
@@ -824,7 +825,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="5">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="I9" s="5">
         <f>SUMIF(G$14:G$24,G9,I$14:I$24)-SUMIF(H$14:H$24,G9,I$14:I$24)</f>
@@ -832,7 +833,7 @@
       </c>
       <c r="J9" s="5">
         <f t="shared" si="0"/>
-        <v>46000</v>
+        <v>46500</v>
       </c>
       <c r="L9" s="7" t="s">
         <v>1</v>
@@ -846,7 +847,7 @@
       </c>
       <c r="O9" s="7">
         <f t="shared" si="1"/>
-        <v>49000</v>
+        <v>49500</v>
       </c>
       <c r="Q9" s="9" t="s">
         <v>1</v>
@@ -860,7 +861,7 @@
       </c>
       <c r="T9" s="9">
         <f t="shared" si="2"/>
-        <v>49000</v>
+        <v>49500</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.3">
@@ -876,23 +877,23 @@
         <v>0</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" si="3"/>
+        <f>SUM(E7:E9)</f>
         <v>48000</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>15</v>
       </c>
       <c r="H10" s="4">
-        <f>SUM(H7:H9)</f>
-        <v>0</v>
+        <f>-H9-H7-H8</f>
+        <v>500</v>
       </c>
       <c r="I10" s="4">
-        <f t="shared" ref="I10" si="4">SUM(I7:I9)</f>
-        <v>-500</v>
+        <f t="shared" ref="I10:J10" si="4">SUM(I7:I9)</f>
+        <v>0</v>
       </c>
       <c r="J10" s="4">
-        <f t="shared" ref="J10" si="5">SUM(J7:J9)</f>
-        <v>48500</v>
+        <f t="shared" si="4"/>
+        <v>47500</v>
       </c>
       <c r="L10" s="6" t="s">
         <v>15</v>
@@ -902,12 +903,12 @@
         <v>0</v>
       </c>
       <c r="N10" s="6">
-        <f t="shared" ref="N10" si="6">SUM(N7:N9)</f>
+        <f t="shared" ref="N10:O10" si="5">SUM(N7:N9)</f>
         <v>-500</v>
       </c>
       <c r="O10" s="6">
-        <f t="shared" ref="O10" si="7">SUM(O7:O9)</f>
-        <v>49000</v>
+        <f t="shared" si="5"/>
+        <v>48000</v>
       </c>
       <c r="Q10" s="8" t="s">
         <v>15</v>
@@ -917,12 +918,12 @@
         <v>0</v>
       </c>
       <c r="S10" s="8">
-        <f t="shared" ref="S10" si="8">SUM(S7:S9)</f>
+        <f t="shared" ref="S10:T10" si="6">SUM(S7:S9)</f>
         <v>0</v>
       </c>
       <c r="T10" s="8">
-        <f t="shared" ref="T10" si="9">SUM(T7:T9)</f>
-        <v>49000</v>
+        <f t="shared" si="6"/>
+        <v>48000</v>
       </c>
     </row>
     <row r="11" spans="2:20" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1012,7 +1013,7 @@
         <v>0</v>
       </c>
       <c r="I14" s="4">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="J14" s="4"/>
       <c r="L14" s="6" t="s">
@@ -1065,4 +1066,580 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{694B896C-C978-4FD0-BD99-54B4F06701F3}">
+  <dimension ref="B1:T15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="13" max="13" width="18.5546875" customWidth="1"/>
+    <col min="14" max="14" width="13.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+    </row>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="4"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" s="6"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="8"/>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2">
+        <f>SUMIF(B$14:B$24,"Asset",D$14:D$24)-SUMIF(C$14:C$24,"Asset",D$14:D$24)</f>
+        <v>48000</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="4">
+        <f>SUMIF(G$14:G$24,"Asset",I$14:I$24)-SUMIF(H$14:H$24,"Asset",I$14:I$24)+D3</f>
+        <v>48500</v>
+      </c>
+      <c r="J3" s="4"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="N3" s="6">
+        <f>SUMIF(L$14:L$24,"Asset",N$14:N$24)-SUMIF(M$14:M$24,"Asset",N$14:N$24)+I3</f>
+        <v>49000</v>
+      </c>
+      <c r="O3" s="6"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="S3" s="8">
+        <f>SUMIF(Q$14:Q$24,"Asset",S$14:S$24)-SUMIF(R$14:R$24,"Asset",S$14:S$24)+N3</f>
+        <v>49000</v>
+      </c>
+      <c r="T3" s="8"/>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="2">
+        <f>D3-E10</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="4">
+        <f>I3-J10</f>
+        <v>-300</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" s="6">
+        <f>N3-O10</f>
+        <v>-300</v>
+      </c>
+      <c r="O4" s="6"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="S4" s="8">
+        <f>S3-T10</f>
+        <v>-300</v>
+      </c>
+      <c r="T4" s="8"/>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="S6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="T6" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <f>SUMIF(B$14:B$24,B7,D$14:D$24)-SUMIF(C$14:C$24,B7,D$14:D$24)</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <f>C7-D7</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="4">
+        <v>-1000</v>
+      </c>
+      <c r="I7" s="4">
+        <f>SUMIF(G$14:G$24,G7,I$14:I$24)-SUMIF(H$14:H$24,G7,I$14:I$24)</f>
+        <v>-1500</v>
+      </c>
+      <c r="J7" s="4">
+        <f>H7-I7+E7</f>
+        <v>500</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M7" s="6">
+        <v>-2000</v>
+      </c>
+      <c r="N7" s="6">
+        <f>SUMIF(L$14:L$24,L7,N$14:N$24)-SUMIF(M$14:M$24,L7,N$14:N$24)</f>
+        <v>-1500</v>
+      </c>
+      <c r="O7" s="6">
+        <f>M7-N7+J7</f>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R7" s="8">
+        <v>0</v>
+      </c>
+      <c r="S7" s="8">
+        <f>SUMIF(Q$14:Q$24,Q7,S$14:S$24)-SUMIF(R$14:R$24,Q7,S$14:S$24)</f>
+        <v>0</v>
+      </c>
+      <c r="T7" s="8">
+        <f>R7-S7+O7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2000</v>
+      </c>
+      <c r="D8" s="2">
+        <f>SUMIF(B$14:B$24,B8,D$14:D$24)-SUMIF(C$14:C$24,B8,D$14:D$24)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <f>C8-D8</f>
+        <v>2000</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="4">
+        <v>500</v>
+      </c>
+      <c r="I8" s="4">
+        <f>SUMIF(G$14:G$24,G8,I$14:I$24)-SUMIF(H$14:H$24,G8,I$14:I$24)</f>
+        <v>1000</v>
+      </c>
+      <c r="J8" s="4">
+        <f t="shared" ref="J8:J9" si="0">H8-I8+E8</f>
+        <v>1500</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M8" s="6">
+        <v>-1000</v>
+      </c>
+      <c r="N8" s="6">
+        <f>SUMIF(L$14:L$24,L8,N$14:N$24)-SUMIF(M$14:M$24,L8,N$14:N$24)</f>
+        <v>1000</v>
+      </c>
+      <c r="O8" s="6">
+        <f t="shared" ref="O8:O9" si="1">M8-N8+J8</f>
+        <v>-500</v>
+      </c>
+      <c r="Q8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="R8" s="8">
+        <v>0</v>
+      </c>
+      <c r="S8" s="8">
+        <f>SUMIF(Q$14:Q$24,Q8,S$14:S$24)-SUMIF(R$14:R$24,Q8,S$14:S$24)</f>
+        <v>0</v>
+      </c>
+      <c r="T8" s="8">
+        <f t="shared" ref="T8:T9" si="2">R8-S8+O8</f>
+        <v>-500</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3">
+        <v>46000</v>
+      </c>
+      <c r="D9" s="3">
+        <f>SUMIF(B$14:B$24,B9,D$14:D$24)-SUMIF(C$14:C$24,B9,D$14:D$24)</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <f>C9-D9</f>
+        <v>46000</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H9" s="5">
+        <v>800</v>
+      </c>
+      <c r="I9" s="5">
+        <f>SUMIF(G$14:G$24,G9,I$14:I$24)-SUMIF(H$14:H$24,G9,I$14:I$24)</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="5">
+        <f t="shared" si="0"/>
+        <v>46800</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M9" s="7">
+        <v>3000</v>
+      </c>
+      <c r="N9" s="7">
+        <f>SUMIF(L$14:L$24,L9,N$14:N$24)-SUMIF(M$14:M$24,L9,N$14:N$24)</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="7">
+        <f t="shared" si="1"/>
+        <v>49800</v>
+      </c>
+      <c r="Q9" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="R9" s="9">
+        <v>0</v>
+      </c>
+      <c r="S9" s="9">
+        <f>SUMIF(Q$14:Q$24,Q9,S$14:S$24)-SUMIF(R$14:R$24,Q9,S$14:S$24)</f>
+        <v>0</v>
+      </c>
+      <c r="T9" s="9">
+        <f t="shared" si="2"/>
+        <v>49800</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2">
+        <f>SUM(C7:C9)</f>
+        <v>48000</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" ref="D10:E10" si="3">SUM(D7:D9)</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="3"/>
+        <v>48000</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="4">
+        <f>SUM(H7:H9)</f>
+        <v>300</v>
+      </c>
+      <c r="I10" s="4">
+        <f t="shared" ref="I10" si="4">SUM(I7:I9)</f>
+        <v>-500</v>
+      </c>
+      <c r="J10" s="4">
+        <f t="shared" ref="J10" si="5">SUM(J7:J9)</f>
+        <v>48800</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="M10" s="6">
+        <f>SUM(M7:M9)</f>
+        <v>0</v>
+      </c>
+      <c r="N10" s="6">
+        <f t="shared" ref="N10" si="6">SUM(N7:N9)</f>
+        <v>-500</v>
+      </c>
+      <c r="O10" s="6">
+        <f t="shared" ref="O10" si="7">SUM(O7:O9)</f>
+        <v>49300</v>
+      </c>
+      <c r="Q10" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="R10" s="8">
+        <f>SUM(R7:R9)</f>
+        <v>0</v>
+      </c>
+      <c r="S10" s="8">
+        <f t="shared" ref="S10" si="8">SUM(S7:S9)</f>
+        <v>0</v>
+      </c>
+      <c r="T10" s="8">
+        <f t="shared" ref="T10" si="9">SUM(T7:T9)</f>
+        <v>49300</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="G13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="4"/>
+      <c r="L13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O13" s="6"/>
+      <c r="Q13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="R13" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="S13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="T13" s="8"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="2">
+        <v>50000</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="G14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14" s="4">
+        <v>1500</v>
+      </c>
+      <c r="J14" s="4"/>
+      <c r="L14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="N14" s="6">
+        <v>1500</v>
+      </c>
+      <c r="O14" s="6"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="2">
+        <v>2000</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="G15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" s="4">
+        <v>1000</v>
+      </c>
+      <c r="J15" s="4"/>
+      <c r="L15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="N15" s="6">
+        <v>1000</v>
+      </c>
+      <c r="O15" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed the budget available calculations. started creating the net worth and available budget card
</commit_message>
<xml_diff>
--- a/Budget Template.xlsx
+++ b/Budget Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Timmy\LocalFiles\Coding\koala-budget-UAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328345AC-A96A-4A8C-834B-BBC27C6EACDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F0B0D5-FA2A-4731-982D-B8ACDCC17696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4FB47142-1B3D-449D-828A-9AE39AA5D3D9}"/>
   </bookViews>
@@ -497,7 +497,7 @@
   <dimension ref="B1:T15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="H3:I4"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -873,7 +873,7 @@
         <v>48000</v>
       </c>
       <c r="D10" s="2">
-        <f t="shared" ref="D10:E10" si="3">SUM(D7:D9)</f>
+        <f t="shared" ref="D10" si="3">SUM(D7:D9)</f>
         <v>0</v>
       </c>
       <c r="E10" s="2">

</xml_diff>

<commit_message>
got budget available card working
</commit_message>
<xml_diff>
--- a/Budget Template.xlsx
+++ b/Budget Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Timmy\LocalFiles\Coding\koala-budget-UAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F0B0D5-FA2A-4731-982D-B8ACDCC17696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19BDD544-FFF2-4FBF-A0DD-D60CF8C5284A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4FB47142-1B3D-449D-828A-9AE39AA5D3D9}"/>
   </bookViews>
@@ -497,7 +497,7 @@
   <dimension ref="B1:T15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>